<commit_message>
Updated handbook with ADCS_crit tlm
</commit_message>
<xml_diff>
--- a/is_1_handbook.xlsx
+++ b/is_1_handbook.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayuresh\Documents\GitHub\IS1_Commissioning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chandranadmin\Documents\IS1_FSW_wksps\cubesat\inspire\hydra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA76399-0A7A-4261-974F-3D1F01E3F927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="inspire_pkt" sheetId="1" r:id="rId1"/>
@@ -10386,7 +10385,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11187,21 +11186,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -12124,23 +12114,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1687"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1430" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1437" sqref="B1437"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="44" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -51442,16 +51425,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S735"/>
   <sheetViews>
-    <sheetView topLeftCell="A207" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F218" sqref="F218"/>
+    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="39.5703125" customWidth="1"/>
     <col min="10" max="10" width="31" customWidth="1"/>
     <col min="11" max="11" width="30.42578125" customWidth="1"/>

</xml_diff>